<commit_message>
add TensorFlow-Lab html file
</commit_message>
<xml_diff>
--- a/Self Driving Car ND.xlsx
+++ b/Self Driving Car ND.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1120" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="145">
   <si>
     <t>Self Driving Car Nano Degree</t>
   </si>
@@ -1229,6 +1229,12 @@
   </si>
   <si>
     <t>3. Read references:</t>
+  </si>
+  <si>
+    <t>https://www.tensorflow.org/get_started/</t>
+  </si>
+  <si>
+    <t>https://www.tensorflow.org/tutorials/layers</t>
   </si>
 </sst>
 </file>
@@ -1335,21 +1341,21 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1628,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1643,11 +1649,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="9" t="s">
         <v>80</v>
       </c>
@@ -1660,12 +1666,12 @@
       <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
@@ -1931,12 +1937,12 @@
       <c r="A30" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
@@ -2101,12 +2107,12 @@
       <c r="A50" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
@@ -2150,52 +2156,52 @@
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
@@ -2206,42 +2212,42 @@
       <c r="D63" s="18"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B67" s="16"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="16"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
     </row>
     <row r="69" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
@@ -2252,533 +2258,490 @@
       <c r="D69" s="18"/>
     </row>
     <row r="70" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="16"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="16"/>
-    </row>
-    <row r="78" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="18" t="s">
+      <c r="A77" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="17"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+    </row>
+    <row r="79" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="16" t="s">
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="16" t="s">
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="19" t="s">
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="19" t="s">
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="16"/>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-    </row>
-    <row r="84" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="18" t="s">
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="17"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+    </row>
+    <row r="86" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="16" t="s">
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B85" s="16"/>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="16"/>
-      <c r="B86" s="16"/>
-      <c r="C86" s="16"/>
-      <c r="D86" s="16"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="16"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="16"/>
-      <c r="D87" s="16"/>
-    </row>
-    <row r="88" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="18" t="s">
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="17"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="17"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+    </row>
+    <row r="90" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B88" s="18"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="16" t="s">
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="B89" s="16"/>
-      <c r="C89" s="16"/>
-      <c r="D89" s="16"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="16" t="s">
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B90" s="16"/>
-      <c r="C90" s="16"/>
-      <c r="D90" s="16"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="19" t="s">
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="19"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="16" t="s">
+      <c r="B93" s="15"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="15"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B92" s="16"/>
-      <c r="C92" s="16"/>
-      <c r="D92" s="16"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="19" t="s">
+      <c r="B94" s="17"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B93" s="19"/>
-      <c r="C93" s="19"/>
-      <c r="D93" s="19"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="16"/>
-      <c r="B94" s="16"/>
-      <c r="C94" s="16"/>
-      <c r="D94" s="16"/>
-    </row>
-    <row r="95" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="18" t="s">
+      <c r="B95" s="15"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="17"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+    </row>
+    <row r="97" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="16" t="s">
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B96" s="16"/>
-      <c r="C96" s="16"/>
-      <c r="D96" s="16"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="19" t="s">
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="20" t="s">
+      <c r="B99" s="15"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="15"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B98" s="20"/>
-      <c r="C98" s="20"/>
-      <c r="D98" s="20"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="20" t="s">
+      <c r="B100" s="16"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="16"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B99" s="20"/>
-      <c r="C99" s="20"/>
-      <c r="D99" s="20"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B100" s="20"/>
-      <c r="C100" s="20"/>
-      <c r="D100" s="20"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="16"/>
       <c r="B101" s="16"/>
       <c r="C101" s="16"/>
       <c r="D101" s="16"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="16"/>
+      <c r="A102" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="B102" s="16"/>
       <c r="C102" s="16"/>
       <c r="D102" s="16"/>
     </row>
-    <row r="103" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="18" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="17"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="17"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
+    </row>
+    <row r="105" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="16" t="s">
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B104" s="16"/>
-      <c r="C104" s="16"/>
-      <c r="D104" s="16"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="16" t="s">
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B105" s="16"/>
-      <c r="C105" s="16"/>
-      <c r="D105" s="16"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="16"/>
-      <c r="B106" s="16"/>
-      <c r="C106" s="16"/>
-      <c r="D106" s="16"/>
-    </row>
-    <row r="107" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="18" t="s">
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="17"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
+    </row>
+    <row r="109" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B107" s="18"/>
-      <c r="C107" s="18"/>
-      <c r="D107" s="18"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="16" t="s">
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B108" s="16"/>
-      <c r="C108" s="16"/>
-      <c r="D108" s="16"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="16" t="s">
+      <c r="B110" s="17"/>
+      <c r="C110" s="17"/>
+      <c r="D110" s="17"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B109" s="16"/>
-      <c r="C109" s="16"/>
-      <c r="D109" s="16"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="16"/>
-      <c r="B110" s="16"/>
-      <c r="C110" s="16"/>
-      <c r="D110" s="16"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="18" t="s">
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="17"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="17"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B111" s="18"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="18"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="16" t="s">
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B112" s="16"/>
-      <c r="C112" s="16"/>
-      <c r="D112" s="16"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="19" t="s">
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B113" s="19"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="19" t="s">
+      <c r="B115" s="15"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="15"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B114" s="19"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="19"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="16"/>
-      <c r="B115" s="16"/>
-      <c r="C115" s="16"/>
-      <c r="D115" s="16"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" s="18" t="s">
+      <c r="B116" s="15"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="17"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="17"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B116" s="18"/>
-      <c r="C116" s="18"/>
-      <c r="D116" s="18"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="16" t="s">
+      <c r="B118" s="18"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="18"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B117" s="16"/>
-      <c r="C117" s="16"/>
-      <c r="D117" s="16"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="16" t="s">
+      <c r="B119" s="17"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="17"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B118" s="16"/>
-      <c r="C118" s="16"/>
-      <c r="D118" s="16"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" s="16"/>
-      <c r="B119" s="16"/>
-      <c r="C119" s="16"/>
-      <c r="D119" s="16"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="18" t="s">
+      <c r="B120" s="17"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="17"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="17"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B120" s="18"/>
-      <c r="C120" s="18"/>
-      <c r="D120" s="18"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="16" t="s">
+      <c r="B122" s="18"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B121" s="16"/>
-      <c r="C121" s="16"/>
-      <c r="D121" s="16"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="16" t="s">
+      <c r="B123" s="17"/>
+      <c r="C123" s="17"/>
+      <c r="D123" s="17"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B122" s="16"/>
-      <c r="C122" s="16"/>
-      <c r="D122" s="16"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" s="19" t="s">
+      <c r="B124" s="17"/>
+      <c r="C124" s="17"/>
+      <c r="D124" s="17"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B123" s="19"/>
-      <c r="C123" s="19"/>
-      <c r="D123" s="19"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="16"/>
-      <c r="B124" s="16"/>
-      <c r="C124" s="16"/>
-      <c r="D124" s="16"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="18" t="s">
+      <c r="B125" s="15"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="17"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="17"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="B125" s="18"/>
-      <c r="C125" s="18"/>
-      <c r="D125" s="18"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" s="16" t="s">
+      <c r="B127" s="18"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="18"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B126" s="16"/>
-      <c r="C126" s="16"/>
-      <c r="D126" s="16"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="16"/>
-      <c r="B127" s="16"/>
-      <c r="C127" s="16"/>
-      <c r="D127" s="16"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="16"/>
-      <c r="B128" s="16"/>
-      <c r="C128" s="16"/>
-      <c r="D128" s="16"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="17"/>
+      <c r="D128" s="17"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="16"/>
-      <c r="B129" s="16"/>
-      <c r="C129" s="16"/>
-      <c r="D129" s="16"/>
+      <c r="A129" s="17"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="17"/>
+      <c r="D129" s="17"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="16"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="16"/>
-      <c r="D130" s="16"/>
+      <c r="A130" s="17"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="16"/>
-      <c r="B131" s="16"/>
-      <c r="C131" s="16"/>
-      <c r="D131" s="16"/>
+      <c r="A131" s="17"/>
+      <c r="B131" s="17"/>
+      <c r="C131" s="17"/>
+      <c r="D131" s="17"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="17"/>
+      <c r="B132" s="17"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="17"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="17"/>
+      <c r="B133" s="17"/>
+      <c r="C133" s="17"/>
+      <c r="D133" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A115:D115"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A122:D122"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A126:D126"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A114:D114"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="A118:D118"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A111:D111"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A104:D104"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A113:D113"/>
+  <mergeCells count="82">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B50:E50"/>
     <mergeCell ref="A67:D67"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A59:D59"/>
@@ -2790,11 +2753,72 @@
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="A65:D65"/>
     <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="A118:D118"/>
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A114:D114"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A79:D79"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E11" r:id="rId1" display="CS231n Convolutional Neural Networks for Visual Recognition"/>
@@ -2852,21 +2876,23 @@
     <hyperlink ref="E19" r:id="rId53"/>
     <hyperlink ref="E25" r:id="rId54"/>
     <hyperlink ref="E1" r:id="rId55"/>
-    <hyperlink ref="A82" r:id="rId56" display="CS231n Convolutional Neural Networks for Visual Recognition"/>
+    <hyperlink ref="A83" r:id="rId56" display="CS231n Convolutional Neural Networks for Visual Recognition"/>
     <hyperlink ref="A76" r:id="rId57" display="Deep Learning, by Goodfellow, Bengio, and Courville."/>
-    <hyperlink ref="A81" r:id="rId58" display="CS 143 Introduction to Computer Vision"/>
+    <hyperlink ref="A82" r:id="rId58" display="CS 143 Introduction to Computer Vision"/>
     <hyperlink ref="A75" r:id="rId59"/>
-    <hyperlink ref="A93" r:id="rId60" display="CS231n Convolutional Neural Networks for Visual Recognition"/>
-    <hyperlink ref="A91" r:id="rId61"/>
-    <hyperlink ref="A97" r:id="rId62"/>
-    <hyperlink ref="A98" r:id="rId63"/>
-    <hyperlink ref="A99" r:id="rId64"/>
-    <hyperlink ref="A100" r:id="rId65"/>
-    <hyperlink ref="A113" r:id="rId66"/>
-    <hyperlink ref="A114" r:id="rId67"/>
-    <hyperlink ref="A123" r:id="rId68"/>
+    <hyperlink ref="A95" r:id="rId60" display="CS231n Convolutional Neural Networks for Visual Recognition"/>
+    <hyperlink ref="A93" r:id="rId61"/>
+    <hyperlink ref="A99" r:id="rId62"/>
+    <hyperlink ref="A100" r:id="rId63"/>
+    <hyperlink ref="A101" r:id="rId64"/>
+    <hyperlink ref="A102" r:id="rId65"/>
+    <hyperlink ref="A115" r:id="rId66"/>
+    <hyperlink ref="A116" r:id="rId67"/>
+    <hyperlink ref="A125" r:id="rId68"/>
     <hyperlink ref="A73" r:id="rId69" display="Computer Vision: Algorithms and Applications"/>
     <hyperlink ref="A74" r:id="rId70"/>
+    <hyperlink ref="A77" r:id="rId71"/>
+    <hyperlink ref="A84" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>